<commit_message>
update files and readme
</commit_message>
<xml_diff>
--- a/mapping_schemes/central/BDI_RES.xlsx
+++ b/mapping_schemes/central/BDI_RES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/npaul/GEM/WIP/africa/data/Africa_Map/Central/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8F0F45-D33D-FE48-A593-39638E38D99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E66C415-F3BA-A249-A818-5A6D6960DB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11020" yWindow="460" windowWidth="16160" windowHeight="17120" firstSheet="1" activeTab="2" xr2:uid="{FDFB1767-49BE-9748-8720-0163DBB19794}"/>
+    <workbookView xWindow="11020" yWindow="460" windowWidth="16160" windowHeight="17120" firstSheet="1" activeTab="1" xr2:uid="{FDFB1767-49BE-9748-8720-0163DBB19794}"/>
   </bookViews>
   <sheets>
     <sheet name="Material_1" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="97">
   <si>
     <t>Urban</t>
   </si>
@@ -4052,10 +4052,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF06C8A-1AE4-2949-8A97-6266F0313480}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4328,35 +4328,35 @@
         <v>2</v>
       </c>
       <c r="D19" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D20" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D21" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -4367,10 +4367,10 @@
         <v>1</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>75</v>
+        <v>13</v>
       </c>
       <c r="D22" s="2">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -4381,35 +4381,35 @@
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="D23" s="2">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
@@ -4417,16 +4417,16 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D26" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -4437,10 +4437,10 @@
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="D27" s="2">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -4451,35 +4451,35 @@
         <v>1</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="D28" s="2">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D29" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D30" s="2">
         <v>1</v>
@@ -4487,13 +4487,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D31" s="2">
         <v>1</v>
@@ -4501,7 +4501,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>1</v>
@@ -4513,81 +4513,108 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
-      <c r="C40" s="3"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="3"/>
@@ -4606,6 +4633,11 @@
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4617,7 +4649,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
@@ -5728,7 +5760,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:C118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>